<commit_message>
finished append to report with concurrency handling mechanism and published
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andreea.ghetu\Documents\UiPath\CSharpChanges\StudioTemplates\REFramework\C#\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UiPath Projects\ListUSAPrivateSchools\ListUSAPrivateSchools_Producer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96902286-4E3C-425E-A0BF-F83C72A8C5F4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBE0C9DD-79F2-4A81-9BB9-C0E764A300EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="18000" windowHeight="9480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="53">
   <si>
     <t>Name</t>
   </si>
@@ -85,13 +85,6 @@
   </si>
   <si>
     <t>logF_BusinessProcessName</t>
-  </si>
-  <si>
-    <t>Framework</t>
-  </si>
-  <si>
-    <t>ProcessABCQueue</t>
-    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>Orchestrator queue Name. The value must match with the queue name defined on Orchestrator.</t>
@@ -161,6 +154,36 @@
   </si>
   <si>
     <t>Folder name. The value must match a folder defined in Orchestrator and queue specified as OrchestratorQueueName should be created in this folder. For classic folders leave the value field empty.</t>
+  </si>
+  <si>
+    <t>ListUSAPrivateSchools_Queue</t>
+  </si>
+  <si>
+    <t>ListUSAPrivateSchools</t>
+  </si>
+  <si>
+    <t>ListUSAPrivateSchools_Producer</t>
+  </si>
+  <si>
+    <t>CurrentReportFilepath</t>
+  </si>
+  <si>
+    <t>Filepath to report created by dispatcher - will be utilised by one or many producers topopulate the single report</t>
+  </si>
+  <si>
+    <t>CurrentReportLock</t>
+  </si>
+  <si>
+    <t>CurrentReportLockAssetName</t>
+  </si>
+  <si>
+    <t>CurrentReportLockAssetFolder</t>
+  </si>
+  <si>
+    <t>FreeLockValue</t>
+  </si>
+  <si>
+    <t>Free</t>
   </si>
 </sst>
 </file>
@@ -212,21 +235,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+  <cellXfs count="5">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -541,10 +559,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z5"/>
+  <dimension ref="A1:Z9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15"/>
@@ -591,36 +609,66 @@
     </row>
     <row r="2" spans="1:26">
       <c r="A2" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>22</v>
+        <v>43</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="45">
-      <c r="A3" s="7" t="s">
-        <v>38</v>
+      <c r="A3" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" t="s">
+        <v>44</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:26">
-      <c r="A4" s="7"/>
+      <c r="A4" s="2"/>
     </row>
     <row r="5" spans="1:26" ht="30">
       <c r="A5" t="s">
         <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>21</v>
+        <v>45</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>24</v>
-      </c>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26">
+      <c r="A7" t="s">
+        <v>49</v>
+      </c>
+      <c r="B7" t="s">
+        <v>48</v>
+      </c>
+      <c r="C7" s="4"/>
+    </row>
+    <row r="8" spans="1:26">
+      <c r="A8" t="s">
+        <v>51</v>
+      </c>
+      <c r="B8" t="s">
+        <v>52</v>
+      </c>
+      <c r="C8" s="4"/>
+    </row>
+    <row r="9" spans="1:26">
+      <c r="A9" t="s">
+        <v>50</v>
+      </c>
+      <c r="B9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C9" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2"/>
@@ -687,24 +735,22 @@
         <v>0</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="45">
-      <c r="A3" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="B3" s="5">
+      <c r="A3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3">
         <v>0</v>
       </c>
-      <c r="C3" s="6" t="s">
-        <v>33</v>
+      <c r="C3" s="3" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:26">
-      <c r="A4" s="5"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="6"/>
+      <c r="C4" s="3"/>
     </row>
     <row r="5" spans="1:26">
       <c r="A5" t="s">
@@ -725,7 +771,7 @@
         <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:26">
@@ -747,7 +793,7 @@
         <v>15</v>
       </c>
       <c r="C9" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:26">
@@ -758,7 +804,7 @@
         <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:26">
@@ -769,56 +815,51 @@
         <v>19</v>
       </c>
       <c r="C11" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:26">
-      <c r="A12" s="5" t="s">
+      <c r="A12" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12" t="s">
         <v>41</v>
       </c>
-      <c r="B12" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="13" spans="1:26">
-      <c r="A13" s="5"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
+      <c r="C12" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="14" spans="1:26">
-      <c r="A14" s="5" t="s">
+      <c r="A14" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14">
+        <v>2</v>
+      </c>
+      <c r="C14" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26">
+      <c r="A15" t="s">
         <v>34</v>
       </c>
-      <c r="B14" s="5">
+      <c r="B15">
         <v>2</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="C15" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="15" spans="1:26">
-      <c r="A15" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="B15" s="5">
-        <v>2</v>
-      </c>
-      <c r="C15" s="5" t="s">
+    <row r="17" spans="1:3" ht="45">
+      <c r="A17" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" ht="45">
-      <c r="A17" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="B17" s="5" t="b">
+      <c r="B17" t="b">
         <v>0</v>
       </c>
-      <c r="C17" s="6" t="s">
-        <v>40</v>
+      <c r="C17" s="3" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -831,8 +872,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -851,7 +892,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>4</v>
@@ -879,7 +920,20 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="2" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D2" t="s">
+        <v>47</v>
+      </c>
+    </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="5" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>